<commit_message>
README perpetuitet and formulas
</commit_message>
<xml_diff>
--- a/02.Lecture/lec02.xlsx
+++ b/02.Lecture/lec02.xlsx
@@ -1,31 +1,203 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\finance\02.Lecture\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C201A0D3-8377-425E-B5A2-2D56D9D22A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Задача 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Человек заключил договор ренты на 20 лет, с ежемесячным платежом 30 тыс.руб. Первый платеж ожидается через месяц. Если стоимость денег равна 10% годовых, то сколько стоит такой договор? Сколько нужно заплатить в момент его заключения?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+количество периодов</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+стоимость денег</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+цена договора в день заключения</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+будующая цена договора</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+месячный платеж</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,11 +221,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +513,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="82.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D2">
+        <v>30000</v>
+      </c>
+      <c r="E2" s="4">
+        <f>PV(C2,B2,D2*12)</f>
+        <v>-3064882.9391130833</v>
+      </c>
+      <c r="F2" s="4">
+        <f>FV(C2,B2,D2*12)</f>
+        <v>-20618999.817572191</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All seminars tasks added
</commit_message>
<xml_diff>
--- a/02.Lecture/lec02.xlsx
+++ b/02.Lecture/lec02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\finance\02.Lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFA4B63-6C88-43E9-8258-2C3ED76D8898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E1B02D-C7CB-42B0-826D-C44832CC5A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Человек заключил договор ренты на 20 лет, с ежемесячным платежом 30 тыс.руб. Первый платеж ожидается через месяц. Если стоимость денег равна 10% годовых, то сколько стоит такой договор? Сколько нужно заплатить в момент его заключения?</t>
   </si>
@@ -272,21 +272,45 @@
   <si>
     <t>Решение. Воспользуемся формулой для приведенной стоимости аннуитета постнумерандо для 4-летнего аннуитета, начинающегося в конце 2 года: PV2 = 100*(1-(1+9%)^(-4))/9% = $324. Чтобы определить текущую стоимость (то есть в момент времени 0), нужно продисконтировать на 2 года: PV0 = PV2 / (1+9%)^2 = $273</t>
   </si>
+  <si>
+    <t>ПЛТ</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Года</t>
+  </si>
+  <si>
+    <t>Приведенная стоимость $100</t>
+  </si>
+  <si>
+    <t>Приведенная (текущая) сумма</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;₽&quot;;[Red]\-#,##0.00\ &quot;₽&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,12 +347,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -343,12 +373,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -356,13 +386,15 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -885,18 +917,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E3BE70-2FC0-472C-AF7E-7ECDDABFD706}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -910,10 +943,13 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>100</v>
       </c>
@@ -923,17 +959,472 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2" s="4">
-        <f>PV(C2,D2,B2)</f>
-        <v>-323.97198770533731</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <f>PMT(C2*4,-2,100,,0)</f>
+        <v>42.372881355932194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7" s="9">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>11</v>
+      </c>
+      <c r="N7" s="9">
+        <v>12</v>
+      </c>
+      <c r="O7">
+        <v>13</v>
+      </c>
+      <c r="P7">
+        <v>14</v>
+      </c>
+      <c r="Q7">
+        <v>15</v>
+      </c>
+      <c r="R7" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>100</v>
+      </c>
+      <c r="C8" s="10">
+        <f>B8-9%</f>
+        <v>99.91</v>
+      </c>
+      <c r="D8" s="10">
+        <f>C8-9%</f>
+        <v>99.82</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" ref="E8:R8" si="0">D8-9%</f>
+        <v>99.72999999999999</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.639999999999986</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.549999999999983</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.45999999999998</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.369999999999976</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.279999999999973</v>
+      </c>
+      <c r="K8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.189999999999969</v>
+      </c>
+      <c r="L8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.099999999999966</v>
+      </c>
+      <c r="M8" s="10">
+        <f t="shared" si="0"/>
+        <v>99.009999999999962</v>
+      </c>
+      <c r="N8" s="10">
+        <f t="shared" si="0"/>
+        <v>98.919999999999959</v>
+      </c>
+      <c r="O8" s="10">
+        <f t="shared" si="0"/>
+        <v>98.829999999999956</v>
+      </c>
+      <c r="P8" s="10">
+        <f t="shared" si="0"/>
+        <v>98.739999999999952</v>
+      </c>
+      <c r="Q8" s="10">
+        <f t="shared" si="0"/>
+        <v>98.649999999999949</v>
+      </c>
+      <c r="R8" s="10">
+        <f t="shared" si="0"/>
+        <v>98.559999999999945</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E9" s="10">
+        <f>E8</f>
+        <v>99.72999999999999</v>
+      </c>
+      <c r="I9" s="10">
+        <f>I8</f>
+        <v>99.369999999999976</v>
+      </c>
+      <c r="M9" s="10">
+        <f>M8</f>
+        <v>99.009999999999962</v>
+      </c>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10">
+        <f>R8</f>
+        <v>98.559999999999945</v>
+      </c>
+      <c r="S9" s="10">
+        <f>SUM(E9:R9)</f>
+        <v>396.66999999999985</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>100*(1+9%)^E11</f>
+        <v>129.50290000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" s="9">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11" s="9">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>11</v>
+      </c>
+      <c r="N11" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="10">
+        <v>100</v>
+      </c>
+      <c r="C12" s="10">
+        <f>B12-B12*9%</f>
+        <v>91</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" ref="D12:N12" si="1">C12-C12*9%</f>
+        <v>82.81</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="1"/>
+        <v>75.357100000000003</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="1"/>
+        <v>68.574961000000002</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="1"/>
+        <v>62.403214509999998</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="1"/>
+        <v>56.786925204100001</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
+        <v>51.676101935730998</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="1"/>
+        <v>47.025252761515205</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" si="1"/>
+        <v>42.792980012978838</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="1"/>
+        <v>38.941611811810745</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="1"/>
+        <v>35.436866748747775</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="1"/>
+        <v>32.247548741360475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="10">
+        <f>E12</f>
+        <v>75.357100000000003</v>
+      </c>
+      <c r="H13" s="10">
+        <f>H12</f>
+        <v>56.786925204100001</v>
+      </c>
+      <c r="K13" s="10">
+        <f>K12</f>
+        <v>42.792980012978838</v>
+      </c>
+      <c r="N13" s="10">
+        <f>N12</f>
+        <v>32.247548741360475</v>
+      </c>
+      <c r="O13" s="10">
+        <f>SUM(N13,K13,H13,E13)</f>
+        <v>207.18455395843932</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C14" s="4">
+        <f>PV(9%,1,B12)</f>
+        <v>-91.743119266055118</v>
+      </c>
+      <c r="D14" s="4">
+        <f>PV(9%,1,C12)</f>
+        <v>-83.486238532110164</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" ref="E14:N14" si="2">PV(9%,1,D12)</f>
+        <v>-75.972477064220243</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="2"/>
+        <v>-69.134954128440427</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="2"/>
+        <v>-62.91280825688078</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="2"/>
+        <v>-57.250655513761515</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="2"/>
+        <v>-52.098096517522976</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="2"/>
+        <v>-47.409267830945907</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="2"/>
+        <v>-43.142433726160775</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="2"/>
+        <v>-39.259614690806302</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="2"/>
+        <v>-35.726249368633738</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="2"/>
+        <v>-32.510886925456695</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <f>E14</f>
+        <v>-75.972477064220243</v>
+      </c>
+      <c r="H15" s="4">
+        <f>H14</f>
+        <v>-57.250655513761515</v>
+      </c>
+      <c r="K15" s="4">
+        <f>K14</f>
+        <v>-43.142433726160775</v>
+      </c>
+      <c r="N15" s="4">
+        <f>N14</f>
+        <v>-32.510886925456695</v>
+      </c>
+      <c r="O15" s="4">
+        <f>SUM(N15,K15,H15,E15)</f>
+        <v>-208.87645322959924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E16" s="4">
+        <f>PV(C2,E11,B12)</f>
+        <v>-253.12946659881763</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" s="9">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+      <c r="J17" s="9">
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="L17">
+        <v>10</v>
+      </c>
+      <c r="M17" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>99.91</v>
+      </c>
+      <c r="D18">
+        <v>99.82</v>
+      </c>
+      <c r="E18">
+        <v>99.72999999999999</v>
+      </c>
+      <c r="F18">
+        <v>99.639999999999986</v>
+      </c>
+      <c r="G18">
+        <v>99.549999999999983</v>
+      </c>
+      <c r="H18">
+        <v>99.45999999999998</v>
+      </c>
+      <c r="I18">
+        <v>99.369999999999976</v>
+      </c>
+      <c r="J18">
+        <v>99.279999999999973</v>
+      </c>
+      <c r="K18">
+        <v>99.189999999999969</v>
+      </c>
+      <c r="L18">
+        <v>99.099999999999966</v>
+      </c>
+      <c r="M18">
+        <v>99.009999999999962</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>D18</f>
+        <v>99.82</v>
+      </c>
+      <c r="G19">
+        <f>G18</f>
+        <v>99.549999999999983</v>
+      </c>
+      <c r="J19">
+        <f>J18</f>
+        <v>99.279999999999973</v>
+      </c>
+      <c r="M19">
+        <v>99.009999999999962</v>
+      </c>
+      <c r="N19">
+        <f>SUM(D19:M19)</f>
+        <v>397.65999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>